<commit_message>
updated students and people
</commit_message>
<xml_diff>
--- a/_data/students.xlsx
+++ b/_data/students.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\idealabasu\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840FCC33-E075-4361-8215-B82B91C2F08A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E81186C-C8C7-43A9-BF9C-99E903B244DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="112">
   <si>
     <t>name</t>
   </si>
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>/assets/images/headshots/brauer2.jpg</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>Spring 2020</t>
   </si>
 </sst>
 </file>
@@ -1209,14 +1215,16 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1297,6 +1305,9 @@
       <c r="P2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="Q2" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="R2" s="1" t="s">
         <v>101</v>
       </c>
@@ -1323,6 +1334,9 @@
       <c r="P3" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="Q3" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="R3" s="1" t="s">
         <v>87</v>
       </c>
@@ -1346,6 +1360,9 @@
       <c r="P4" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="Q4" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="R4" s="1" t="s">
         <v>107</v>
       </c>
@@ -1372,6 +1389,9 @@
       <c r="P5" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="Q5" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>88</v>
       </c>
@@ -1427,8 +1447,14 @@
       <c r="L7" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="M7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P7" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>109</v>
@@ -1453,6 +1479,9 @@
       <c r="P8" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="Q8" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="R8" s="1" t="s">
         <v>90</v>
       </c>
@@ -1467,11 +1496,11 @@
       <c r="L9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="P9" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>103</v>
@@ -1673,6 +1702,9 @@
       <c r="P16" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="Q16" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="R16" s="1" t="s">
         <v>95</v>
       </c>
@@ -1693,8 +1725,11 @@
       <c r="I17" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="O17" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P17" s="1" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="R17" s="1" t="s">
         <v>96</v>
@@ -1719,6 +1754,9 @@
       <c r="P18" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="Q18" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="R18" s="1" t="s">
         <v>97</v>
       </c>
@@ -1742,6 +1780,9 @@
       <c r="P19" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="Q19" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="R19" s="1" t="s">
         <v>103</v>
       </c>
@@ -1762,6 +1803,9 @@
       <c r="M20" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="O20" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="P20" s="1" t="s">
         <v>56</v>
       </c>
@@ -1791,6 +1835,9 @@
       <c r="P21" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="Q21" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="R21" s="1" t="s">
         <v>100</v>
       </c>
@@ -1808,6 +1855,9 @@
       <c r="P22" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="Q22" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="R22" s="1" t="s">
         <v>103</v>
       </c>
@@ -1824,6 +1874,9 @@
       </c>
       <c r="P23" s="1" t="s">
         <v>56</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>103</v>

</xml_diff>